<commit_message>
Create test cases in two Excel files
Create 10 cases of Container boats in teset_container.xlsx and 20 cases of tugboats in test_tug.xlsx.
</commit_message>
<xml_diff>
--- a/web/WBTBSsystem/test_container.xlsx
+++ b/web/WBTBSsystem/test_container.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Y3_GRP\Web-Based-Tug-Boat-Scheduling-System\web\WBTBSsystem\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\YSY\Desktop\GRP\CW\Web-Based-Tug-Boat-Scheduling-System\web\WBTBSsystem\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C18F18E-D9F0-4BD7-99F6-C42C71A113E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFD3398E-6BB9-47E1-82F0-21F17ABC64F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4020" yWindow="3315" windowWidth="16200" windowHeight="11250" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,37 +20,95 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="24">
   <si>
     <t>ContainerBoatID</t>
   </si>
   <si>
+    <t>Country</t>
+  </si>
+  <si>
+    <t>ArrivalTime</t>
+  </si>
+  <si>
+    <t>China</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Action</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>INBOUND</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>BerthID</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>CN0001</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>CN0002</t>
+  </si>
+  <si>
+    <t>CN0003</t>
+  </si>
+  <si>
+    <t>CN0004</t>
+  </si>
+  <si>
+    <t>US0001</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>US0002</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>RU0001</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>JP0001</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>KR0001</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>MY0001</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
     <t>Tonnage</t>
-  </si>
-  <si>
-    <t>Country</t>
-  </si>
-  <si>
-    <t>ArrivalTime</t>
-  </si>
-  <si>
-    <t>China</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Action</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>INBOUND</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>BerthID</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>CN0001</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>OUTBOUND</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>America</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Russia</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Japan</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Korea</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Malaysia</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -435,73 +493,239 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:F5"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="13.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.5546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="16.44140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.5" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="16.5" style="5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2">
+        <v>100</v>
+      </c>
+      <c r="C2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="F1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="D2" s="3">
+        <v>45388.375</v>
+      </c>
+      <c r="E2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>8</v>
       </c>
-      <c r="B2">
+      <c r="B3">
+        <v>200</v>
+      </c>
+      <c r="C3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" s="3">
+        <v>45388.416666666664</v>
+      </c>
+      <c r="E3" t="s">
+        <v>5</v>
+      </c>
+      <c r="F3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4">
         <v>300</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D4" s="3">
+        <v>45389.385416666664</v>
+      </c>
+      <c r="E4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5">
+        <v>400</v>
+      </c>
+      <c r="C5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D5" s="3">
+        <v>45388.416666666664</v>
+      </c>
+      <c r="E5" t="s">
+        <v>5</v>
+      </c>
+      <c r="F5">
         <v>4</v>
       </c>
-      <c r="D2" s="3">
-        <v>45357.916666666664</v>
-      </c>
-      <c r="E2" t="s">
+    </row>
+    <row r="6" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6">
+        <v>255</v>
+      </c>
+      <c r="C6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D6" s="3">
+        <v>45389.625</v>
+      </c>
+      <c r="E6" t="s">
+        <v>18</v>
+      </c>
+      <c r="F6">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7">
+        <v>437</v>
+      </c>
+      <c r="C7" t="s">
+        <v>19</v>
+      </c>
+      <c r="D7" s="3">
+        <v>45388.666666666664</v>
+      </c>
+      <c r="E7" t="s">
+        <v>5</v>
+      </c>
+      <c r="F7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8">
+        <v>368</v>
+      </c>
+      <c r="C8" t="s">
+        <v>20</v>
+      </c>
+      <c r="D8" s="3">
+        <v>45388.541666666664</v>
+      </c>
+      <c r="E8" t="s">
+        <v>5</v>
+      </c>
+      <c r="F8">
         <v>6</v>
       </c>
-      <c r="F2">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3"/>
-      <c r="D3"/>
-      <c r="E3"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B4"/>
-      <c r="D4"/>
-      <c r="E4"/>
-    </row>
-    <row r="5" spans="1:6" ht="15" x14ac:dyDescent="0.3">
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
+    </row>
+    <row r="9" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9">
+        <v>120</v>
+      </c>
+      <c r="C9" t="s">
+        <v>21</v>
+      </c>
+      <c r="D9" s="3">
+        <v>45388.541666666664</v>
+      </c>
+      <c r="E9" t="s">
+        <v>5</v>
+      </c>
+      <c r="F9">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10">
+        <v>167</v>
+      </c>
+      <c r="C10" t="s">
+        <v>22</v>
+      </c>
+      <c r="D10" s="3">
+        <v>45388.5</v>
+      </c>
+      <c r="E10" t="s">
+        <v>5</v>
+      </c>
+      <c r="F10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>16</v>
+      </c>
+      <c r="B11">
+        <v>288</v>
+      </c>
+      <c r="C11" t="s">
+        <v>23</v>
+      </c>
+      <c r="D11" s="3">
+        <v>45389.458333333336</v>
+      </c>
+      <c r="E11" t="s">
+        <v>18</v>
+      </c>
+      <c r="F11">
+        <v>2</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>

</xml_diff>